<commit_message>
Server & App completed
</commit_message>
<xml_diff>
--- a/src/server/database/data.xlsx
+++ b/src/server/database/data.xlsx
@@ -6,6 +6,28 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -396,13 +418,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="str">
-        <v>Milk</v>
+        <v>plastic</v>
       </c>
       <c r="C2" t="str">
-        <v>xxxxx677</v>
+        <v>0000000000001</v>
       </c>
       <c r="D2" t="str">
-        <v>paper</v>
+        <v>plastic</v>
       </c>
     </row>
     <row r="3">
@@ -410,13 +432,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="str">
-        <v>Beer</v>
+        <v>paper</v>
       </c>
       <c r="C3" t="str">
-        <v>xxxxx678</v>
+        <v>0000000000002</v>
       </c>
       <c r="D3" t="str">
-        <v>glass</v>
+        <v>paper</v>
       </c>
     </row>
     <row r="4">
@@ -424,13 +446,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="str">
-        <v>Beakers</v>
+        <v>glass</v>
       </c>
       <c r="C4" t="str">
-        <v>xxxxx679</v>
+        <v>0000000000003</v>
       </c>
       <c r="D4" t="str">
-        <v>paper</v>
+        <v>glass</v>
       </c>
     </row>
     <row r="5">
@@ -438,18 +460,102 @@
         <v>3</v>
       </c>
       <c r="B5" t="str">
-        <v>Banana</v>
+        <v>Calve knoflook saus</v>
       </c>
       <c r="C5" t="str">
-        <v>xxxxx680</v>
+        <v>8720182255563</v>
       </c>
       <c r="D5" t="str">
-        <v>organic</v>
+        <v>plastic</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>4</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Verstegen paprikapoeder</v>
+      </c>
+      <c r="C6" t="str">
+        <v>8712200856104</v>
+      </c>
+      <c r="D6" t="str">
+        <v>glass</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>5</v>
+      </c>
+      <c r="B7" t="str">
+        <v>AH tomatenpuree</v>
+      </c>
+      <c r="C7" t="str">
+        <v>8059602910011</v>
+      </c>
+      <c r="D7" t="str">
+        <v>plastic</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>6</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Calve pindakaas stukjes</v>
+      </c>
+      <c r="C8" t="str">
+        <v>8711200430925</v>
+      </c>
+      <c r="D8" t="str">
+        <v>glass</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>7</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Cup a soup tomaat</v>
+      </c>
+      <c r="C9" t="str">
+        <v>5711327460348</v>
+      </c>
+      <c r="D9" t="str">
+        <v>glass</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>8</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Pickwick winterglow</v>
+      </c>
+      <c r="C10" t="str">
+        <v>8711000008881</v>
+      </c>
+      <c r="D10" t="str">
+        <v>paper</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>9</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Coca Cola blik</v>
+      </c>
+      <c r="C11" t="str">
+        <v>5449000008046</v>
+      </c>
+      <c r="D11" t="str">
+        <v>paper</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>